<commit_message>
Update Excel file 2024-08-31 22:26:23.354972
</commit_message>
<xml_diff>
--- a/Android.xlsx
+++ b/Android.xlsx
@@ -472,7 +472,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y27"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>2024-08-30 12:15:48</t>
+          <t>2024-08-31 22:26:05</t>
         </is>
       </c>
       <c r="R24" t="inlineStr"/>
@@ -1379,7 +1379,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>2024-08-21 20:17:10</t>
+          <t>2024-08-30 12:15:48</t>
         </is>
       </c>
       <c r="R25" t="inlineStr"/>
@@ -1414,7 +1414,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>2024-08-21 20:16:45</t>
+          <t>2024-08-21 20:17:10</t>
         </is>
       </c>
       <c r="R26" t="inlineStr"/>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>2024-08-21 20:15:50</t>
+          <t>2024-08-21 20:16:45</t>
         </is>
       </c>
       <c r="R27" t="inlineStr"/>
@@ -1461,6 +1461,72 @@
       <c r="X27" t="inlineStr"/>
       <c r="Y27" t="inlineStr"/>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>hdfc</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>2024-08-21 20:15:50</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Broadband</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="inlineStr"/>
+      <c r="T29" t="inlineStr"/>
+      <c r="U29" t="inlineStr"/>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
+      <c r="X29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>